<commit_message>
Removed printLn functions, added multiple assertions, change tests structure, added simple methods for WebElements
</commit_message>
<xml_diff>
--- a/xlsx/Test.xlsx
+++ b/xlsx/Test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="104">
   <si>
     <t>login</t>
   </si>
@@ -295,46 +295,43 @@
     <t>32d23ffg</t>
   </si>
   <si>
+    <t>Petrovich2088</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
     <t>isPassed</t>
   </si>
   <si>
-    <t>Petrovich2088</t>
-  </si>
-  <si>
-    <t>w</t>
+    <t>passed</t>
+  </si>
+  <si>
+    <t>Email *</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>Имя *</t>
   </si>
   <si>
     <t>Пользователь *</t>
   </si>
   <si>
-    <t>failed</t>
-  </si>
-  <si>
-    <t>Email *</t>
+    <t>Фамилия *</t>
+  </si>
+  <si>
+    <t>Подтверждение *</t>
   </si>
   <si>
     <t>Пароль *</t>
   </si>
   <si>
-    <t>Подтверждение *</t>
-  </si>
-  <si>
-    <t>passed</t>
-  </si>
-  <si>
-    <t>Имя *</t>
-  </si>
-  <si>
-    <t>Фамилия *</t>
-  </si>
-  <si>
     <t>IRC nick</t>
-  </si>
-  <si>
-    <t>Поиск</t>
   </si>
 </sst>
 </file>
@@ -669,7 +666,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -717,10 +714,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>90</v>
@@ -735,7 +732,7 @@
         <v>57</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>81</v>
@@ -1125,36 +1122,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4">
@@ -1162,7 +1159,7 @@
         <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
@@ -1170,39 +1167,351 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
         <v>100</v>
+      </c>
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>101</v>
+      </c>
+      <c r="B47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>102</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited some boolean checks
</commit_message>
<xml_diff>
--- a/xlsx/Test.xlsx
+++ b/xlsx/Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
   <si>
     <t>login</t>
   </si>
@@ -237,34 +237,46 @@
     <t>GaluaPulemet6</t>
   </si>
   <si>
-    <t>GaluaPulemet6@gmail.com</t>
-  </si>
-  <si>
     <t>GaluaPulemet7</t>
   </si>
   <si>
-    <t>GaluaPulemet7@gmail.com</t>
-  </si>
-  <si>
     <t>GaluaPulemet8</t>
   </si>
   <si>
-    <t>GaluaPulemet8@gmail.com</t>
-  </si>
-  <si>
     <t>GaluaPulemet9</t>
   </si>
   <si>
-    <t>GaluaPulemet9@gmail.com</t>
-  </si>
-  <si>
-    <t>Magnifikate77</t>
-  </si>
-  <si>
-    <t>Magnifikate77@gmail.com</t>
-  </si>
-  <si>
     <t>Petrovich200777</t>
+  </si>
+  <si>
+    <t>GaluaPulemet72</t>
+  </si>
+  <si>
+    <t>GaluaPulemet82</t>
+  </si>
+  <si>
+    <t>GaluaPulemet92</t>
+  </si>
+  <si>
+    <t>Magnifikate772</t>
+  </si>
+  <si>
+    <t>GaluaPulemet72@gmail.com</t>
+  </si>
+  <si>
+    <t>GaluaPulemet82@gmail.com</t>
+  </si>
+  <si>
+    <t>GaluaPulemet92@gmail.com</t>
+  </si>
+  <si>
+    <t>Magnifikate772@gmail.com</t>
+  </si>
+  <si>
+    <t>GaluaPulemet64</t>
+  </si>
+  <si>
+    <t>GaluaPulemet64@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -611,7 +623,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -659,10 +671,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>26</v>
@@ -688,10 +700,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
@@ -706,10 +718,10 @@
         <v>70</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -717,10 +729,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>26</v>
@@ -735,10 +747,10 @@
         <v>70</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -746,10 +758,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>26</v>
@@ -764,10 +776,10 @@
         <v>70</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -778,7 +790,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>28</v>
@@ -793,7 +805,7 @@
         <v>43</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
removed useless methods from RegisterPage, CheckInputsAtOnce
</commit_message>
<xml_diff>
--- a/xlsx/Test.xlsx
+++ b/xlsx/Test.xlsx
@@ -249,34 +249,34 @@
     <t>Petrovich200777</t>
   </si>
   <si>
-    <t>GaluaPulemet72</t>
-  </si>
-  <si>
-    <t>GaluaPulemet82</t>
-  </si>
-  <si>
-    <t>GaluaPulemet92</t>
-  </si>
-  <si>
-    <t>Magnifikate772</t>
-  </si>
-  <si>
-    <t>GaluaPulemet72@gmail.com</t>
-  </si>
-  <si>
-    <t>GaluaPulemet82@gmail.com</t>
-  </si>
-  <si>
-    <t>GaluaPulemet92@gmail.com</t>
-  </si>
-  <si>
     <t>Magnifikate772@gmail.com</t>
   </si>
   <si>
-    <t>GaluaPulemet64</t>
-  </si>
-  <si>
-    <t>GaluaPulemet64@gmail.com</t>
+    <t>GaluaPulemet644</t>
+  </si>
+  <si>
+    <t>GaluaPulemet724</t>
+  </si>
+  <si>
+    <t>GaluaPulemet824</t>
+  </si>
+  <si>
+    <t>GaluaPulemet924</t>
+  </si>
+  <si>
+    <t>Magnifikate7724</t>
+  </si>
+  <si>
+    <t>GaluaPulemet644@gmail.com</t>
+  </si>
+  <si>
+    <t>GaluaPulemet724@gmail.com</t>
+  </si>
+  <si>
+    <t>GaluaPulemet824@gmail.com</t>
+  </si>
+  <si>
+    <t>GaluaPulemet924@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -671,10 +671,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>26</v>
@@ -700,10 +700,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>26</v>
@@ -729,10 +729,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>26</v>
@@ -758,10 +758,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>26</v>
@@ -787,10 +787,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>28</v>

</xml_diff>